<commit_message>
feat: Implementação completa de homologação WPP, Reabertura e Aprovisionamentos
- WPP: Normalização de telefones, CEPs e datas; enriquecimento com Base Analítica
- Reabertura: Formato XLSX, agrupamento por CPF, validação de número da ordem (formato 1-XXXXXXXXXXXXX)
- Aprovisionamentos: Filtros avançados, colunas ICCID, Tipo de Venda, Status da entrega
- Validação de formato de número da ordem com fallback para Numero OS da Base Analítica
- Limpeza de arquivos temporários de validação
- Scripts .bat para geração e validação de homologação
</commit_message>
<xml_diff>
--- a/triggers.xlsx
+++ b/triggers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dspin\OneDrive\Documents\Projetos_python\3F_Qigger_DBGerenciador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9769D4-0372-4DF5-9C79-4A8ADAEC1CD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B2EF86-4B0B-4262-9F1D-3F25B3FD44FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43080" yWindow="11910" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$73</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$77</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="63">
   <si>
     <t>REGRA_ID</t>
   </si>
@@ -85,9 +85,6 @@
     <t>ERRO SIEBEL</t>
   </si>
   <si>
-    <t>VALIDAR GROSS</t>
-  </si>
-  <si>
     <t>LIBERACAO BONUS</t>
   </si>
   <si>
@@ -106,9 +103,6 @@
     <t>CANCELADO A PEDIDO CLIENTE</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>Portado</t>
   </si>
   <si>
@@ -158,9 +152,6 @@
   </si>
   <si>
     <t>DIVERGEGECIA DOADORA</t>
-  </si>
-  <si>
-    <t>CPF - INCENTIVO NOVA LINHA</t>
   </si>
   <si>
     <t>Portabillidade de Número Vago</t>
@@ -596,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M73"/>
+  <dimension ref="A1:M77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G71" sqref="G1:G71"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.4"/>
@@ -677,10 +668,10 @@
         <v>16</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="M2" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.4">
@@ -694,13 +685,13 @@
         <v>18</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="K3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="M3" s="2">
         <v>2</v>
@@ -714,16 +705,16 @@
         <v>13</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="K4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="M4" s="2">
         <v>2</v>
@@ -734,25 +725,25 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>17</v>
@@ -766,25 +757,25 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" s="2" t="s">
+      <c r="L6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="M6" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.4">
@@ -792,25 +783,25 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>17</v>
@@ -824,25 +815,25 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8" s="2" t="s">
+      <c r="L8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="M8" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.4">
@@ -850,25 +841,25 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="L9" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.4">
@@ -876,28 +867,28 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="L10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="M10" s="2">
-        <v>2</v>
+        <v>45</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.4">
@@ -905,25 +896,25 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J11" s="2" t="s">
+      <c r="L11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="M11" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.4">
@@ -931,25 +922,25 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="L12" s="2" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.4">
@@ -957,25 +948,25 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K13" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="L13" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M13" s="2">
         <v>2</v>
@@ -986,31 +977,31 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J14" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="K14" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>45</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.4">
@@ -1018,25 +1009,25 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="D15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K15" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="L15" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M15" s="2">
         <v>2</v>
@@ -1047,31 +1038,31 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.4">
@@ -1079,28 +1070,28 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M17" s="2">
         <v>2</v>
@@ -1111,31 +1102,31 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L18" s="2" t="s">
         <v>45</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.4">
@@ -1143,28 +1134,28 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="D19" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M19" s="2">
         <v>2</v>
@@ -1175,31 +1166,31 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K20" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="L20" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="M20" s="2">
-        <v>2</v>
+        <v>45</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.4">
@@ -1207,25 +1198,25 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K21" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J21" s="2" t="s">
+      <c r="L21" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K21" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L21" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="M21" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.4">
@@ -1233,31 +1224,31 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="D22" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>45</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.4">
@@ -1265,28 +1256,28 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M23" s="2">
         <v>2</v>
@@ -1300,7 +1291,7 @@
         <v>13</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>15</v>
@@ -1309,7 +1300,7 @@
         <v>16</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="M24" s="2">
         <v>2</v>
@@ -1320,28 +1311,28 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M25" s="2">
         <v>2</v>
@@ -1352,28 +1343,28 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="D26" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M26" s="2">
         <v>2</v>
@@ -1384,28 +1375,28 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M27" s="2">
         <v>2</v>
@@ -1416,31 +1407,31 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C28" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K28" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="K28" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="L28" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.4">
@@ -1448,31 +1439,31 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J29" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="K29" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L29" s="2" t="s">
         <v>45</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.4">
@@ -1480,31 +1471,31 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L30" s="2" t="s">
         <v>45</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.4">
@@ -1512,28 +1503,28 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M31" s="2">
         <v>2</v>
@@ -1544,31 +1535,31 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C32" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K32" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K32" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="L32" s="2" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.4">
@@ -1576,25 +1567,25 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D33" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K33" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="L33" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M33" s="2">
         <v>2</v>
@@ -1605,31 +1596,31 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="D34" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L34" s="2" t="s">
         <v>45</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.4">
@@ -1637,25 +1628,25 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J35" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L35" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K35" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L35" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="M35" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.4">
@@ -1663,25 +1654,25 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M36" s="2">
         <v>2</v>
@@ -1692,25 +1683,25 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D37" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K37" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F37" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="L37" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M37" s="2">
         <v>2</v>
@@ -1721,31 +1712,31 @@
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="D38" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.4">
@@ -1753,31 +1744,31 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J39" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="K39" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.4">
@@ -1785,31 +1776,31 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J40" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="K40" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.4">
@@ -1817,31 +1808,31 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J41" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="K41" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.4">
@@ -1852,7 +1843,7 @@
         <v>13</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J42" s="2" t="s">
         <v>15</v>
@@ -1861,7 +1852,7 @@
         <v>16</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="M42" s="2">
         <v>2</v>
@@ -1872,28 +1863,28 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M43" s="2">
         <v>2</v>
@@ -1904,25 +1895,25 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K44" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J44" s="2" t="s">
+      <c r="L44" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K44" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L44" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="M44" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.4">
@@ -1930,25 +1921,25 @@
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J45" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L45" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K45" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L45" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="M45" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.4">
@@ -1956,25 +1947,25 @@
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D46" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K46" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F46" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J46" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="K46" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="L46" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M46" s="2">
         <v>2</v>
@@ -1985,25 +1976,25 @@
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J47" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C47" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J47" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="K47" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="M47" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.4">
@@ -2011,31 +2002,31 @@
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J48" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J48" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="K48" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L48" s="2" t="s">
         <v>45</v>
       </c>
       <c r="M48" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.4">
@@ -2043,28 +2034,28 @@
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M49" s="2">
         <v>2</v>
@@ -2075,25 +2066,25 @@
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D50" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K50" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F50" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J50" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="K50" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="L50" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M50" s="2">
         <v>2</v>
@@ -2104,31 +2095,31 @@
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L51" s="2" t="s">
         <v>45</v>
       </c>
       <c r="M51" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.4">
@@ -2136,25 +2127,25 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J52" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K52" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L52" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K52" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L52" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="M52" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.4">
@@ -2162,31 +2153,31 @@
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C53" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J53" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K53" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J53" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="K53" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="L53" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="M53" s="2">
-        <v>2</v>
+        <v>45</v>
+      </c>
+      <c r="M53" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.4">
@@ -2194,22 +2185,22 @@
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J54" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L54" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="M54" s="2">
-        <v>2</v>
+        <v>20</v>
+      </c>
+      <c r="M54" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.4">
@@ -2217,19 +2208,10 @@
         <v>54</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="J55" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="K55" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L55" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="M55" s="2">
-        <v>2</v>
+        <v>60</v>
+      </c>
+      <c r="M55" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.4">
@@ -2237,22 +2219,22 @@
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J56" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C56" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J56" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="K56" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="L56" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="M56" s="2">
         <v>1</v>
@@ -2263,22 +2245,22 @@
         <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J57" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C57" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J57" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="K57" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="L57" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="M57" s="2">
         <v>1</v>
@@ -2289,28 +2271,28 @@
         <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="M58" s="2">
         <v>2</v>
@@ -2321,22 +2303,22 @@
         <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J59" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C59" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J59" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="K59" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="M59" s="2">
         <v>1</v>
@@ -2347,22 +2329,22 @@
         <v>59</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="L60" s="2" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="M60" s="2">
         <v>2</v>
@@ -2373,22 +2355,22 @@
         <v>60</v>
       </c>
       <c r="B61" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J61" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C61" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J61" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="K61" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="L61" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="M61" s="2">
         <v>1</v>
@@ -2399,22 +2381,22 @@
         <v>61</v>
       </c>
       <c r="B62" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J62" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C62" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F62" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J62" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="K62" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="L62" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="M62" s="2">
         <v>1</v>
@@ -2425,31 +2407,31 @@
         <v>62</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J63" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L63" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="M63" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.4">
@@ -2457,22 +2439,22 @@
         <v>63</v>
       </c>
       <c r="B64" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J64" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C64" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F64" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J64" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="K64" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="L64" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="M64" s="2">
         <v>1</v>
@@ -2483,31 +2465,31 @@
         <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J65" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L65" s="2" t="s">
         <v>45</v>
       </c>
       <c r="M65" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.4">
@@ -2515,28 +2497,28 @@
         <v>65</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J66" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="L66" s="2" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="M66" s="2">
         <v>2</v>
@@ -2547,22 +2529,22 @@
         <v>66</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J67" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="L67" s="2" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="M67" s="2">
         <v>2</v>
@@ -2573,22 +2555,22 @@
         <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J68" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C68" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J68" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="K68" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="L68" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="M68" s="2">
         <v>1</v>
@@ -2599,22 +2581,22 @@
         <v>68</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J69" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="L69" s="2" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="M69" s="2">
         <v>2</v>
@@ -2625,22 +2607,22 @@
         <v>69</v>
       </c>
       <c r="B70" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J70" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C70" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J70" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="K70" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="L70" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="M70" s="2">
         <v>1</v>
@@ -2651,28 +2633,28 @@
         <v>70</v>
       </c>
       <c r="B71" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J71" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C71" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F71" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J71" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="K71" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L71" s="2" t="s">
         <v>45</v>
       </c>
       <c r="M71" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.4">
@@ -2680,22 +2662,22 @@
         <v>71</v>
       </c>
       <c r="B72" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J72" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C72" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J72" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="K72" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="L72" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="M72" s="2">
         <v>1</v>
@@ -2706,28 +2688,121 @@
         <v>72</v>
       </c>
       <c r="B73" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J73" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C73" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J73" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="K73" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="L73" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="M73" s="2">
         <v>1</v>
       </c>
     </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A74" s="2">
+        <v>73</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J74" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K74" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="L74" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A75" s="2">
+        <v>74</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J75" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K75" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="L75" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A76" s="2">
+        <v>75</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J76" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K76" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="L76" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A77" s="2">
+        <v>76</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J77" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K77" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="L77" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:M77" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>